<commit_message>
Android Fragment and Mongo DB
ModifyOrderDialog, DateHelper at android and server http connection at
Mongo DB
</commit_message>
<xml_diff>
--- a/Hurryhurry_DBTable.xlsx
+++ b/Hurryhurry_DBTable.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E6095A-153D-491D-9A16-8899FAA6A02C}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>

</xml_diff>